<commit_message>
last update for noww
</commit_message>
<xml_diff>
--- a/03_Output/Exercise c/c_Japan.xlsx
+++ b/03_Output/Exercise c/c_Japan.xlsx
@@ -360,12 +360,12 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>NACE</t>
+          <t>nace</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>year</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -412,14 +412,6 @@
       </c>
       <c r="B2">
         <v>1995</v>
-      </c>
-      <c r="C2">
-        <v>-2.967825831896319</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
       </c>
       <c r="F2">
         <v>-0.08513590375708824</v>

</xml_diff>